<commit_message>
Adiciona checklist de controle de processo da sprint1
</commit_message>
<xml_diff>
--- a/1. Gerenciamento de Projeto/GP - Checklist Verificacao de Projeto v1.0.xlsx
+++ b/1. Gerenciamento de Projeto/GP - Checklist Verificacao de Projeto v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20475" windowHeight="8415" activeTab="4"/>
+    <workbookView windowWidth="28785" windowHeight="13065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -566,7 +566,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="126">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -601,6 +601,9 @@
     <t>Nome do Verificador:</t>
   </si>
   <si>
+    <t>Lucas de Moraes Corrêa</t>
+  </si>
+  <si>
     <t>O ideal é que o índice de aderência ao processo tenha entre 70 e 100%</t>
   </si>
   <si>
@@ -631,22 +634,31 @@
     <t>Existe template para documento não previsto no SpinOff?</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Desenvolvimento - Requisitos</t>
+  </si>
+  <si>
+    <t>visão</t>
+  </si>
+  <si>
+    <t>O artefato foi criado com o template atual e armazenado na pasta correta da estrutura do projeto?</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>O objetivo, os problemas  e as necessidades do cliente estão claras?</t>
+  </si>
+  <si>
+    <t>As necessidades foram descritas como histórias de usuário?</t>
+  </si>
+  <si>
     <t>Não</t>
   </si>
   <si>
-    <t>Desenvolvimento - Requisitos</t>
-  </si>
-  <si>
-    <t>visão</t>
-  </si>
-  <si>
-    <t>O artefato foi criado com o template atual e armazenado na pasta correta da estrutura do projeto?</t>
-  </si>
-  <si>
-    <t>O objetivo, os problemas  e as necessidades do cliente estão claras?</t>
-  </si>
-  <si>
-    <t>As necessidades foram descritas como histórias de usuário?</t>
+    <t>Utilizamos uma notação em mapa mental, e no documento descrevemos cada funcionalidade</t>
   </si>
   <si>
     <t>Fornece uma visão geral do sistema de forma clara e objetiva?</t>
@@ -939,10 +951,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -1036,6 +1048,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1043,15 +1063,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1064,9 +1086,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1089,7 +1110,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1120,14 +1141,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1137,14 +1150,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1167,6 +1172,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1180,18 +1192,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1224,25 +1236,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1260,19 +1272,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1284,13 +1296,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1302,25 +1314,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,7 +1338,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1344,13 +1350,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1380,7 +1392,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1392,19 +1404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1577,26 +1577,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1619,8 +1619,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1630,6 +1630,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1649,21 +1664,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1677,152 +1677,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1844,7 +1844,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1907,6 +1907,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1916,6 +1919,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -1931,7 +1937,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2079,10 +2085,10 @@
             <c:numRef>
               <c:f>Indicadores!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.703703703703704</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2151,7 +2157,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2575,63 +2581,63 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="24.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="39" style="36" customWidth="1"/>
+    <col min="2" max="2" width="39" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" spans="1:2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="39"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="42">
         <f>'Ver-Iniciação1'!$F$2</f>
+        <v>0.703703703703704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="42">
+        <f>'Ver-Elaboração1'!$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="40" t="e">
-        <f>'Ver-Elaboração1'!$F$2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40" t="e">
+      <c r="B5" s="42">
         <f>'Ver-Construção1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="40" t="e">
+      <c r="B6" s="42">
         <f>'Ver-Transição1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:2">
@@ -2642,6 +2648,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2652,8 +2659,8 @@
   <sheetPr/>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -2681,14 +2688,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="C2" s="32">
+        <v>44474</v>
+      </c>
       <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="9">
-        <f>COUNTIF(D5:D52,"Sim")/(COUNTA(D5:D52)-COUNTIF(D5:D52,"NA"))</f>
-        <v>0</v>
+        <f>IFERROR(COUNTIF(D5:D52,"Sim")/(COUNTA(D5:D52)-COUNTIF(D5:D52,"NA")),0)</f>
+        <v>0.703703703703704</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:6">
@@ -2696,66 +2705,68 @@
         <v>10</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
     <row r="4" ht="15" spans="1:6">
       <c r="A4" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="E4" s="34" t="s">
         <v>17</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" ht="15" spans="1:6">
+    <row r="6" spans="1:6">
       <c r="A6" s="25"/>
       <c r="B6" s="21">
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:6">
       <c r="A7" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -2763,38 +2774,46 @@
     </row>
     <row r="8" ht="15" customHeight="1" spans="1:6">
       <c r="A8" s="20"/>
-      <c r="B8" s="34">
+      <c r="B8" s="35">
         <v>2</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" ht="15" spans="1:6">
+    <row r="9" spans="1:6">
       <c r="A9" s="20"/>
       <c r="B9" s="21">
         <v>3</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="23"/>
+        <v>27</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" ht="15" spans="1:6">
+    <row r="10" ht="60" spans="1:6">
       <c r="A10" s="20"/>
       <c r="B10" s="21">
         <v>4</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>30</v>
+      </c>
       <c r="F10" s="22"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="15" spans="1:6">
@@ -2803,21 +2822,25 @@
         <v>5</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="23"/>
+        <v>31</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" ht="16.5" customHeight="1" spans="1:6">
+    <row r="12" ht="30" spans="1:6">
       <c r="A12" s="20"/>
       <c r="B12" s="21">
         <v>6</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
@@ -2825,21 +2848,23 @@
       <c r="A13" s="20"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
     </row>
-    <row r="14" ht="15" spans="1:6">
+    <row r="14" spans="1:6">
       <c r="A14" s="20"/>
       <c r="B14" s="26">
         <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
     </row>
@@ -2849,9 +2874,11 @@
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
@@ -2861,9 +2888,11 @@
         <v>9</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
     </row>
@@ -2873,9 +2902,11 @@
         <v>10</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
@@ -2885,9 +2916,11 @@
         <v>11</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
     </row>
@@ -2895,7 +2928,7 @@
       <c r="A19" s="20"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -2907,9 +2940,11 @@
         <v>12</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="23"/>
+        <v>39</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
@@ -2919,9 +2954,11 @@
         <v>13</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="23"/>
+        <v>40</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
@@ -2929,33 +2966,37 @@
       <c r="A22" s="20"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" ht="15" spans="1:6">
+    <row r="23" spans="1:6">
       <c r="A23" s="20"/>
       <c r="B23" s="26">
         <v>14</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" ht="15" spans="1:6">
+    <row r="24" spans="1:6">
       <c r="A24" s="20"/>
       <c r="B24" s="21">
         <v>15</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="23"/>
+        <v>42</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
     </row>
@@ -2963,57 +3004,63 @@
       <c r="A25" s="20"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" ht="15" spans="1:6">
+    <row r="26" spans="1:6">
       <c r="A26" s="20"/>
       <c r="B26" s="26">
         <v>16</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" ht="15" spans="1:6">
+    <row r="27" spans="1:6">
       <c r="A27" s="20"/>
       <c r="B27" s="21">
         <v>17</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
     </row>
     <row r="28" ht="15" spans="1:6">
       <c r="A28" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" ht="15" spans="1:6">
+    <row r="29" spans="1:6">
       <c r="A29" s="20"/>
       <c r="B29" s="26">
         <v>18</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
     </row>
@@ -3021,45 +3068,51 @@
       <c r="A30" s="20"/>
       <c r="B30" s="17"/>
       <c r="C30" s="18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" ht="15" spans="1:6">
+    <row r="31" spans="1:6">
       <c r="A31" s="20"/>
       <c r="B31" s="26">
         <v>18</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" ht="15" spans="1:6">
+    <row r="32" spans="1:6">
       <c r="A32" s="20"/>
       <c r="B32" s="21">
         <v>19</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="23"/>
+        <v>48</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" ht="15" spans="1:6">
+    <row r="33" spans="1:6">
       <c r="A33" s="20"/>
       <c r="B33" s="21">
         <v>20</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
     </row>
@@ -3067,81 +3120,93 @@
       <c r="A34" s="20"/>
       <c r="B34" s="17"/>
       <c r="C34" s="18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" ht="15" spans="1:6">
+    <row r="35" spans="1:6">
       <c r="A35" s="20"/>
       <c r="B35" s="26">
         <v>21</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" ht="15" spans="1:6">
+    <row r="36" spans="1:6">
       <c r="A36" s="20"/>
       <c r="B36" s="21">
         <v>22</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="23"/>
+        <v>51</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" ht="15" spans="1:6">
+    <row r="37" spans="1:6">
       <c r="A37" s="20"/>
       <c r="B37" s="21">
         <v>23</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="23"/>
+        <v>52</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" ht="15" spans="1:6">
+    <row r="38" spans="1:6">
       <c r="A38" s="20"/>
       <c r="B38" s="21">
         <v>24</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="23"/>
+        <v>53</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" ht="15" spans="1:6">
+    <row r="39" spans="1:6">
       <c r="A39" s="20"/>
       <c r="B39" s="21">
         <v>25</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" ht="15" spans="1:6">
+    <row r="40" spans="1:6">
       <c r="A40" s="20"/>
       <c r="B40" s="21">
         <v>26</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
     </row>
@@ -3151,43 +3216,49 @@
         <v>27</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" ht="15" spans="1:6">
+    <row r="42" spans="1:6">
       <c r="A42" s="20"/>
       <c r="B42" s="21">
         <v>28</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="23"/>
+        <v>57</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" ht="15" spans="1:6">
+    <row r="43" spans="1:6">
       <c r="A43" s="30"/>
       <c r="B43" s="21">
         <v>29</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="23"/>
+        <v>58</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
     </row>
     <row r="44" ht="15" customHeight="1" spans="1:6">
       <c r="A44" s="29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="19"/>
@@ -3198,34 +3269,40 @@
       <c r="B45" s="26">
         <v>30</v>
       </c>
-      <c r="C45" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="23"/>
+      <c r="C45" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
     </row>
-    <row r="46" ht="15" spans="1:6">
+    <row r="46" spans="1:6">
       <c r="A46" s="30"/>
       <c r="B46" s="21">
         <v>31</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
     </row>
-    <row r="47" ht="15" spans="1:6">
+    <row r="47" spans="1:6">
       <c r="A47" s="30"/>
       <c r="B47" s="21">
         <v>32</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="23"/>
+        <v>63</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
     </row>
@@ -3235,9 +3312,11 @@
         <v>33</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="23"/>
+        <v>64</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
     </row>
@@ -3245,45 +3324,51 @@
       <c r="A49" s="30"/>
       <c r="B49" s="17"/>
       <c r="C49" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
     </row>
-    <row r="50" ht="15" spans="1:6">
+    <row r="50" spans="1:6">
       <c r="A50" s="30"/>
       <c r="B50" s="26">
         <v>34</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" ht="15" spans="1:6">
+    <row r="51" spans="1:6">
       <c r="A51" s="30"/>
       <c r="B51" s="21">
         <v>35</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D51" s="23"/>
+        <v>66</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
     </row>
-    <row r="52" ht="15" spans="1:6">
+    <row r="52" spans="1:6">
       <c r="A52" s="30"/>
       <c r="B52" s="21">
         <v>36</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="23"/>
+        <v>67</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>22</v>
+      </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
     </row>
@@ -3300,12 +3385,13 @@
     <mergeCell ref="A44:A52"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6;D8:D12;D14:D18;D20:D21;D23:D24;D26:D27;D29:D33;D35:D43;D45:D48;D50:D52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6;D8:D12;D14:D18;D20:D21;D23:D24;D26:D27;D29:D30;D31:D33;D35:D43;D45:D48;D50:D52">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageSetup paperSize="9" scale="48" orientation="landscape" horizontalDpi="600"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -3350,9 +3436,9 @@
         <v>9</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="9" t="e">
-        <f>COUNTIF(D5:D48,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+      <c r="F2" s="9">
+        <f>IFERROR(COUNTIF(D5:D48,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA")),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:6">
@@ -3362,38 +3448,38 @@
       <c r="B3" s="5"/>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
     <row r="4" ht="15" spans="1:6">
       <c r="A4" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -3405,7 +3491,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="22"/>
@@ -3415,7 +3501,7 @@
       <c r="A7" s="20"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -3427,7 +3513,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="22"/>
@@ -3437,7 +3523,7 @@
       <c r="A9" s="20"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -3449,7 +3535,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="22"/>
@@ -3461,7 +3547,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="22"/>
@@ -3473,7 +3559,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="22"/>
@@ -3485,7 +3571,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="22"/>
@@ -3495,7 +3581,7 @@
       <c r="A14" s="20"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -3507,7 +3593,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="22"/>
@@ -3517,7 +3603,7 @@
       <c r="A16" s="20"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -3529,7 +3615,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="22"/>
@@ -3537,11 +3623,11 @@
     </row>
     <row r="18" ht="15" customHeight="1" spans="1:6">
       <c r="A18" s="16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="19"/>
@@ -3553,7 +3639,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="22"/>
@@ -3565,7 +3651,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="22"/>
@@ -3577,19 +3663,19 @@
         <v>11</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" ht="45" spans="1:6">
+    <row r="22" ht="30" spans="1:6">
       <c r="A22" s="20"/>
       <c r="B22" s="21">
         <v>12</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="22"/>
@@ -3601,7 +3687,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="22"/>
@@ -3611,7 +3697,7 @@
       <c r="A24" s="20"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="19"/>
@@ -3623,7 +3709,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="22"/>
@@ -3635,7 +3721,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="22"/>
@@ -3643,11 +3729,11 @@
     </row>
     <row r="27" ht="15" spans="1:6">
       <c r="A27" s="16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="19"/>
@@ -3659,7 +3745,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="22"/>
@@ -3671,19 +3757,19 @@
         <v>18</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" ht="30" spans="1:6">
+    <row r="30" ht="15" spans="1:6">
       <c r="A30" s="20"/>
       <c r="B30" s="21">
         <v>19</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="22"/>
@@ -3695,7 +3781,7 @@
         <v>20</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="22"/>
@@ -3707,7 +3793,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="22"/>
@@ -3719,7 +3805,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="22"/>
@@ -3727,11 +3813,11 @@
     </row>
     <row r="34" ht="15" spans="1:6">
       <c r="A34" s="28" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D34" s="24"/>
       <c r="E34" s="19"/>
@@ -3743,7 +3829,7 @@
         <v>23</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="22"/>
@@ -3755,7 +3841,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="22"/>
@@ -3767,7 +3853,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="22"/>
@@ -3779,7 +3865,7 @@
         <v>26</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="22"/>
@@ -3791,7 +3877,7 @@
         <v>27</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="22"/>
@@ -3803,7 +3889,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="22"/>
@@ -3811,11 +3897,11 @@
     </row>
     <row r="41" ht="15" customHeight="1" spans="1:6">
       <c r="A41" s="29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="19"/>
@@ -3827,7 +3913,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="22"/>
@@ -3839,7 +3925,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D43" s="23"/>
       <c r="E43" s="22"/>
@@ -3851,7 +3937,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D44" s="23"/>
       <c r="E44" s="22"/>
@@ -3861,7 +3947,7 @@
       <c r="A45" s="30"/>
       <c r="B45" s="17"/>
       <c r="C45" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="19"/>
@@ -3873,7 +3959,7 @@
         <v>32</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="22"/>
@@ -3885,7 +3971,7 @@
         <v>33</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D47" s="23"/>
       <c r="E47" s="22"/>
@@ -3897,7 +3983,7 @@
         <v>34</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D48" s="23"/>
       <c r="E48" s="22"/>
@@ -3922,6 +4008,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -3933,7 +4020,7 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -3966,9 +4053,9 @@
         <v>9</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="9" t="e">
-        <f>COUNTIF(D5:D51,"Sim")/(COUNTA(D5:D51)-COUNTIF(D5:D51,"NA"))</f>
-        <v>#DIV/0!</v>
+      <c r="F2" s="9">
+        <f>IFERROR(COUNTIF(D5:D51,"Sim")/(COUNTA(D5:D51)-COUNTIF(D5:D51,"NA")),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:6">
@@ -3978,38 +4065,38 @@
       <c r="B3" s="5"/>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
     <row r="4" ht="15" spans="1:6">
       <c r="A4" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -4021,7 +4108,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="22"/>
@@ -4031,7 +4118,7 @@
       <c r="A7" s="20"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -4043,7 +4130,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="22"/>
@@ -4053,7 +4140,7 @@
       <c r="A9" s="20"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -4065,7 +4152,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="22"/>
@@ -4077,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="22"/>
@@ -4089,7 +4176,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="22"/>
@@ -4099,7 +4186,7 @@
       <c r="A13" s="20"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -4111,7 +4198,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="22"/>
@@ -4121,7 +4208,7 @@
       <c r="A15" s="20"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -4133,7 +4220,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="22"/>
@@ -4141,11 +4228,11 @@
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="19"/>
@@ -4157,7 +4244,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="22"/>
@@ -4169,7 +4256,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="22"/>
@@ -4179,7 +4266,7 @@
       <c r="A20" s="20"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="19"/>
@@ -4191,7 +4278,7 @@
         <v>10</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="22"/>
@@ -4199,11 +4286,11 @@
     </row>
     <row r="22" ht="15" spans="1:6">
       <c r="A22" s="16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="19"/>
@@ -4215,7 +4302,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="22"/>
@@ -4227,7 +4314,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="22"/>
@@ -4239,7 +4326,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="22"/>
@@ -4251,7 +4338,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="22"/>
@@ -4263,7 +4350,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="22"/>
@@ -4275,7 +4362,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="22"/>
@@ -4283,11 +4370,11 @@
     </row>
     <row r="29" ht="15" spans="1:6">
       <c r="A29" s="16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="19"/>
@@ -4299,7 +4386,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="22"/>
@@ -4311,7 +4398,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="22"/>
@@ -4323,7 +4410,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="22"/>
@@ -4335,7 +4422,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="22"/>
@@ -4347,19 +4434,19 @@
         <v>21</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" ht="30" spans="1:6">
+    <row r="35" ht="15" spans="1:6">
       <c r="A35" s="20"/>
       <c r="B35" s="21">
         <v>22</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="22"/>
@@ -4371,7 +4458,7 @@
         <v>23</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="22"/>
@@ -4379,11 +4466,11 @@
     </row>
     <row r="37" ht="15" spans="1:6">
       <c r="A37" s="28" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="19"/>
@@ -4395,7 +4482,7 @@
         <v>24</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="22"/>
@@ -4407,7 +4494,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="22"/>
@@ -4419,7 +4506,7 @@
         <v>26</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="22"/>
@@ -4431,7 +4518,7 @@
         <v>27</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="22"/>
@@ -4443,7 +4530,7 @@
         <v>28</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="22"/>
@@ -4455,7 +4542,7 @@
         <v>29</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D43" s="23"/>
       <c r="E43" s="22"/>
@@ -4463,11 +4550,11 @@
     </row>
     <row r="44" ht="15" customHeight="1" spans="1:6">
       <c r="A44" s="29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="19"/>
@@ -4479,7 +4566,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="22"/>
@@ -4491,7 +4578,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="22"/>
@@ -4503,7 +4590,7 @@
         <v>32</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D47" s="23"/>
       <c r="E47" s="22"/>
@@ -4513,7 +4600,7 @@
       <c r="A48" s="30"/>
       <c r="B48" s="17"/>
       <c r="C48" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="19"/>
@@ -4525,7 +4612,7 @@
         <v>33</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="22"/>
@@ -4537,7 +4624,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D50" s="23"/>
       <c r="E50" s="22"/>
@@ -4549,7 +4636,7 @@
         <v>35</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D51" s="23"/>
       <c r="E51" s="22"/>
@@ -4603,6 +4690,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -4613,8 +4701,8 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -4647,9 +4735,9 @@
         <v>9</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="9" t="e">
-        <f>COUNTIF(D5:D50,"Sim")/(COUNTA(D5:D50)-COUNTIF(D5:D50,"NA"))</f>
-        <v>#DIV/0!</v>
+      <c r="F2" s="9">
+        <f>IFERROR(COUNTIF(D5:D50,"Sim")/(COUNTA(D5:D50)-COUNTIF(D5:D50,"NA")),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:6">
@@ -4659,38 +4747,38 @@
       <c r="B3" s="5"/>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
     <row r="4" ht="15" spans="1:6">
       <c r="A4" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -4702,7 +4790,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="22"/>
@@ -4712,7 +4800,7 @@
       <c r="A7" s="20"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -4724,7 +4812,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="22"/>
@@ -4734,7 +4822,7 @@
       <c r="A9" s="20"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -4746,7 +4834,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="22"/>
@@ -4758,7 +4846,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="22"/>
@@ -4770,7 +4858,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="22"/>
@@ -4780,7 +4868,7 @@
       <c r="A13" s="20"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -4792,7 +4880,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="22"/>
@@ -4802,7 +4890,7 @@
       <c r="A15" s="20"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -4814,7 +4902,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="22"/>
@@ -4822,11 +4910,11 @@
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="19"/>
@@ -4838,7 +4926,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="22"/>
@@ -4846,23 +4934,23 @@
     </row>
     <row r="19" ht="15" customHeight="1" spans="1:6">
       <c r="A19" s="16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" ht="30" spans="1:6">
+    <row r="20" ht="15" spans="1:6">
       <c r="A20" s="20"/>
       <c r="B20" s="21">
         <v>9</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="22"/>
@@ -4874,7 +4962,7 @@
         <v>10</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="22"/>
@@ -4886,7 +4974,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="22"/>
@@ -4898,7 +4986,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="22"/>
@@ -4910,7 +4998,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="22"/>
@@ -4918,11 +5006,11 @@
     </row>
     <row r="25" ht="15" spans="1:6">
       <c r="A25" s="16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="19"/>
@@ -4934,19 +5022,19 @@
         <v>14</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" ht="30" spans="1:6">
+    <row r="27" ht="15" spans="1:6">
       <c r="A27" s="20"/>
       <c r="B27" s="21">
         <v>15</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="22"/>
@@ -4958,7 +5046,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="22"/>
@@ -4966,11 +5054,11 @@
     </row>
     <row r="29" s="1" customFormat="1" ht="15" customHeight="1" spans="1:6">
       <c r="A29" s="16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="19"/>
@@ -4982,7 +5070,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="22"/>
@@ -4994,7 +5082,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="22"/>
@@ -5004,7 +5092,7 @@
       <c r="A32" s="20"/>
       <c r="B32" s="17"/>
       <c r="C32" s="18" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="19"/>
@@ -5016,7 +5104,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="22"/>
@@ -5028,7 +5116,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="22"/>
@@ -5036,11 +5124,11 @@
     </row>
     <row r="35" ht="15" spans="1:6">
       <c r="A35" s="28" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="19"/>
@@ -5052,7 +5140,7 @@
         <v>19</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="22"/>
@@ -5064,7 +5152,7 @@
         <v>20</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="22"/>
@@ -5076,7 +5164,7 @@
         <v>21</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="22"/>
@@ -5088,7 +5176,7 @@
         <v>22</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="22"/>
@@ -5100,19 +5188,19 @@
         <v>23</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" ht="30" spans="1:6">
+    <row r="41" ht="15" spans="1:6">
       <c r="A41" s="28"/>
       <c r="B41" s="21">
         <v>24</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="22"/>
@@ -5124,7 +5212,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="22"/>
@@ -5132,11 +5220,11 @@
     </row>
     <row r="43" ht="15" customHeight="1" spans="1:6">
       <c r="A43" s="29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="19"/>
@@ -5148,7 +5236,7 @@
         <v>26</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D44" s="23"/>
       <c r="E44" s="22"/>
@@ -5160,7 +5248,7 @@
         <v>27</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="22"/>
@@ -5172,7 +5260,7 @@
         <v>28</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="22"/>
@@ -5182,7 +5270,7 @@
       <c r="A47" s="30"/>
       <c r="B47" s="17"/>
       <c r="C47" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="19"/>
@@ -5194,7 +5282,7 @@
         <v>29</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D48" s="23"/>
       <c r="E48" s="22"/>
@@ -5206,7 +5294,7 @@
         <v>30</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="22"/>
@@ -5218,7 +5306,7 @@
         <v>31</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D50" s="23"/>
       <c r="E50" s="22"/>

</xml_diff>